<commit_message>
working on login/removed unnecessary files
</commit_message>
<xml_diff>
--- a/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
+++ b/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimne/Documents/4CHIF/SYP/Projekt/webshop-jasmin/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Schule\SYP\Project Repo\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDDC7C0-7ACE-AF4F-A3F2-59957E4FAA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B43B16-BC2F-4E84-BAB5-07B1D25E0CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenaufzeichnung" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Stundenaufzeichnung Sommersemester</t>
   </si>
@@ -284,6 +282,9 @@
   </si>
   <si>
     <t>Login mit netlify</t>
+  </si>
+  <si>
+    <t>Working on login system</t>
   </si>
 </sst>
 </file>
@@ -760,95 +761,95 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1130,77 +1131,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN40"/>
+  <dimension ref="A1:AN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J12" zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X36" sqref="X36:Z36"/>
+    <sheetView tabSelected="1" topLeftCell="J22" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.33203125" customWidth="1"/>
-    <col min="32" max="32" width="13.6640625" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.36328125" customWidth="1"/>
+    <col min="23" max="23" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.36328125" customWidth="1"/>
+    <col min="32" max="32" width="13.6328125" customWidth="1"/>
+    <col min="33" max="33" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-    </row>
-    <row r="2" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-    </row>
-    <row r="3" spans="1:18" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="J3" s="71" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="J3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
@@ -1208,7 +1209,7 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="15"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1218,10 +1219,10 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="92"/>
+      <c r="F4" s="71"/>
       <c r="I4" s="13"/>
       <c r="J4" s="16"/>
       <c r="K4" s="12"/>
@@ -1233,11 +1234,11 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="13"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="91" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="91"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="3">
         <v>44620</v>
       </c>
@@ -1277,11 +1278,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="91" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="91"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="3">
         <v>44634</v>
       </c>
@@ -1314,11 +1315,11 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="23"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="91"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="46">
@@ -1342,11 +1343,11 @@
       <c r="Q7" s="12"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="91"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="46">
@@ -1373,11 +1374,11 @@
       <c r="Q8" s="12"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="91" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="46">
@@ -1406,7 +1407,7 @@
         <v>4.513888888888884E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I10" s="13"/>
       <c r="J10" s="16">
         <v>10</v>
@@ -1429,7 +1430,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1460,12 +1461,12 @@
         <v>0.66249999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="I12" s="13"/>
       <c r="J12" s="16">
         <v>12</v>
@@ -1481,7 +1482,7 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I13" s="13"/>
       <c r="J13" s="16">
         <v>13</v>
@@ -1497,7 +1498,7 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1517,10 +1518,10 @@
       <c r="G14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="85" t="s">
+      <c r="H14" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="86"/>
+      <c r="I14" s="82"/>
       <c r="J14" s="16">
         <v>14</v>
       </c>
@@ -1535,11 +1536,11 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="79" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="80"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="19">
         <f>SUM(J23:J31)</f>
         <v>0.53819444444444442</v>
@@ -1554,11 +1555,11 @@
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="87">
+      <c r="H15" s="83">
         <f>SUM(C15:G15)</f>
         <v>1.0888888888888888</v>
       </c>
-      <c r="I15" s="88"/>
+      <c r="I15" s="84"/>
       <c r="J15" s="16">
         <v>17</v>
       </c>
@@ -1573,11 +1574,11 @@
       <c r="Q15" s="12"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="81" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="19">
         <f>SUM(J23:J29)</f>
         <v>0.3923611111111111</v>
@@ -1592,11 +1593,11 @@
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="74">
+      <c r="H16" s="85">
         <f>SUM(C16:G16)</f>
         <v>1.1083333333333336</v>
       </c>
-      <c r="I16" s="75"/>
+      <c r="I16" s="86"/>
       <c r="J16" s="16">
         <v>44</v>
       </c>
@@ -1616,11 +1617,11 @@
       <c r="Q16" s="12"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A17" s="93" t="s">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A17" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="94"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="19">
         <f>SUM(AD23:AD28)</f>
         <v>0.4472222222222223</v>
@@ -1635,11 +1636,11 @@
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="74">
+      <c r="H17" s="85">
         <f>SUM(C17:G17)</f>
         <v>1.2284722222222224</v>
       </c>
-      <c r="I17" s="75"/>
+      <c r="I17" s="86"/>
       <c r="J17" s="16">
         <v>22</v>
       </c>
@@ -1654,11 +1655,11 @@
       <c r="Q17" s="12"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:40" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="83" t="s">
+    <row r="18" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="84"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="20">
         <f>SUM(AN23:AN27)</f>
         <v>0.2749999999999998</v>
@@ -1673,11 +1674,11 @@
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="76">
+      <c r="H18" s="87">
         <f>SUM(C18:G18)</f>
         <v>0.7520833333333331</v>
       </c>
-      <c r="I18" s="77"/>
+      <c r="I18" s="88"/>
       <c r="J18" s="28">
         <v>23</v>
       </c>
@@ -1692,14 +1693,14 @@
       <c r="Q18" s="9"/>
       <c r="R18" s="17"/>
     </row>
-    <row r="19" spans="1:40" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="H19" s="12"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A21" s="78"/>
-      <c r="B21" s="78"/>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1712,11 +1713,11 @@
       <c r="D22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
       <c r="H22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1736,11 +1737,11 @@
       <c r="N22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O22" s="65" t="s">
+      <c r="O22" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="65"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
       <c r="R22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1760,11 +1761,11 @@
       <c r="X22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Y22" s="65" t="s">
+      <c r="Y22" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="Z22" s="65"/>
-      <c r="AA22" s="65"/>
+      <c r="Z22" s="66"/>
+      <c r="AA22" s="66"/>
       <c r="AB22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1784,11 +1785,11 @@
       <c r="AH22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AI22" s="65" t="s">
+      <c r="AI22" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="AJ22" s="65"/>
-      <c r="AK22" s="65"/>
+      <c r="AJ22" s="66"/>
+      <c r="AK22" s="66"/>
       <c r="AL22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="35" t="s">
         <v>3</v>
       </c>
@@ -1809,11 +1810,11 @@
       <c r="C23" s="30">
         <v>44622</v>
       </c>
-      <c r="E23" s="73" t="s">
+      <c r="E23" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="31">
         <v>0.49305555555555558</v>
       </c>
@@ -1834,11 +1835,11 @@
         <v>44626</v>
       </c>
       <c r="N23" s="43"/>
-      <c r="O23" s="66" t="s">
+      <c r="O23" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="66"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
       <c r="R23" s="31">
         <v>0.79166666666666663</v>
       </c>
@@ -1858,11 +1859,11 @@
       <c r="W23" s="30">
         <v>44626</v>
       </c>
-      <c r="Y23" s="66" t="s">
+      <c r="Y23" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="Z23" s="66"/>
-      <c r="AA23" s="66"/>
+      <c r="Z23" s="65"/>
+      <c r="AA23" s="65"/>
       <c r="AB23" s="31">
         <v>0.79166666666666663</v>
       </c>
@@ -1882,11 +1883,11 @@
       <c r="AG23" s="30">
         <v>44626</v>
       </c>
-      <c r="AI23" s="66" t="s">
+      <c r="AI23" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="AJ23" s="66"/>
-      <c r="AK23" s="66"/>
+      <c r="AJ23" s="65"/>
+      <c r="AK23" s="65"/>
       <c r="AL23" s="31">
         <v>0.79166666666666663</v>
       </c>
@@ -1898,15 +1899,15 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C24" s="30">
         <v>44626</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="31">
         <v>0.79166666666666663</v>
       </c>
@@ -1973,15 +1974,15 @@
         <v>6.4583333333333215E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C25" s="30">
         <v>44627</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
       <c r="H25" s="11">
         <v>0.33333333333333331</v>
       </c>
@@ -2016,10 +2017,10 @@
       <c r="W25" s="30">
         <v>44630</v>
       </c>
-      <c r="Y25" s="68" t="s">
+      <c r="Y25" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="Z25" s="68"/>
+      <c r="Z25" s="89"/>
       <c r="AB25" s="11">
         <v>0.75</v>
       </c>
@@ -2049,15 +2050,15 @@
         <v>7.1527777777777746E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C26" s="30">
         <v>44627</v>
       </c>
-      <c r="E26" s="66" t="s">
+      <c r="E26" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
       <c r="H26" s="11">
         <v>0.83333333333333337</v>
       </c>
@@ -2092,11 +2093,11 @@
       <c r="W26" s="30">
         <v>44630</v>
       </c>
-      <c r="Y26" s="68" t="s">
+      <c r="Y26" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="Z26" s="68"/>
-      <c r="AA26" s="68"/>
+      <c r="Z26" s="89"/>
+      <c r="AA26" s="89"/>
       <c r="AB26" s="11">
         <v>0.875</v>
       </c>
@@ -2129,18 +2130,18 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C27" s="30">
         <v>44629</v>
       </c>
       <c r="D27">
         <v>44.47</v>
       </c>
-      <c r="E27" s="66" t="s">
+      <c r="E27" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
       <c r="H27" s="11">
         <v>0.49305555555555558</v>
       </c>
@@ -2157,11 +2158,11 @@
       <c r="N27" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="O27" s="68" t="s">
+      <c r="O27" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="P27" s="68"/>
-      <c r="Q27" s="68"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="89"/>
       <c r="R27" s="11">
         <v>0.76041666666666663</v>
       </c>
@@ -2212,18 +2213,18 @@
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C28" s="30">
         <v>44629</v>
       </c>
       <c r="D28">
         <v>44.47</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="E28" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
       <c r="H28" s="11">
         <v>0.72916666666666663</v>
       </c>
@@ -2299,18 +2300,18 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C29" s="30">
         <v>44630</v>
       </c>
       <c r="D29">
         <v>44.47</v>
       </c>
-      <c r="E29" s="66" t="s">
+      <c r="E29" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
       <c r="H29" s="11">
         <v>0.625</v>
       </c>
@@ -2351,11 +2352,11 @@
       <c r="W29" s="30">
         <v>44634</v>
       </c>
-      <c r="Y29" s="70" t="s">
+      <c r="Y29" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="Z29" s="70"/>
-      <c r="AA29" s="70"/>
+      <c r="Z29" s="90"/>
+      <c r="AA29" s="90"/>
       <c r="AB29" s="36">
         <v>0.64583333333333337</v>
       </c>
@@ -2383,18 +2384,18 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C30" s="30">
         <v>44631</v>
       </c>
       <c r="D30">
         <v>44.47</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="E30" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
       <c r="H30" s="11">
         <v>0.625</v>
       </c>
@@ -2434,11 +2435,11 @@
         <v>44635</v>
       </c>
       <c r="X30" s="12"/>
-      <c r="Y30" s="67" t="s">
+      <c r="Y30" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="Z30" s="67"/>
-      <c r="AA30" s="67"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="91"/>
       <c r="AB30" s="36">
         <v>0.625</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="41">
@@ -2475,11 +2476,11 @@
       <c r="D31" s="5">
         <v>44.46</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E31" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
       <c r="H31" s="39">
         <v>0.8125</v>
       </c>
@@ -2510,11 +2511,11 @@
         <v>44637</v>
       </c>
       <c r="X31" s="12"/>
-      <c r="Y31" s="67" t="s">
+      <c r="Y31" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="Z31" s="67"/>
-      <c r="AA31" s="67"/>
+      <c r="Z31" s="91"/>
+      <c r="AA31" s="91"/>
       <c r="AB31" s="36">
         <v>0.83333333333333337</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>6.6666666666666652E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>78</v>
       </c>
@@ -2558,11 +2559,11 @@
       <c r="D32" s="27">
         <v>46</v>
       </c>
-      <c r="E32" s="73" t="s">
+      <c r="E32" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
       <c r="H32" s="11">
         <v>0.64583333333333337</v>
       </c>
@@ -2629,18 +2630,18 @@
         <v>0.11875000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C33" s="30">
         <v>44636</v>
       </c>
       <c r="D33">
         <v>47</v>
       </c>
-      <c r="E33" s="66" t="s">
+      <c r="E33" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
       <c r="H33" s="11">
         <v>0.49305555555555558</v>
       </c>
@@ -2673,11 +2674,11 @@
       <c r="W33" s="30">
         <v>44641</v>
       </c>
-      <c r="Y33" s="68" t="s">
+      <c r="Y33" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="Z33" s="68"/>
-      <c r="AA33" s="68"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="89"/>
       <c r="AB33" s="11">
         <v>0.33333333333333331</v>
       </c>
@@ -2708,18 +2709,18 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C34" s="30">
         <v>44637</v>
       </c>
       <c r="D34">
         <v>26</v>
       </c>
-      <c r="E34" s="66" t="s">
+      <c r="E34" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
       <c r="H34" s="11">
         <v>0.75</v>
       </c>
@@ -2746,17 +2747,17 @@
         <v>0.70208333333333339</v>
       </c>
       <c r="T34" s="38">
-        <f t="shared" ref="T34:T40" si="7">S34-R34</f>
+        <f t="shared" ref="T34:T41" si="7">S34-R34</f>
         <v>0.11875000000000002</v>
       </c>
       <c r="W34" s="30">
         <v>44642</v>
       </c>
-      <c r="Y34" s="68" t="s">
+      <c r="Y34" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="Z34" s="68"/>
-      <c r="AA34" s="68"/>
+      <c r="Z34" s="89"/>
+      <c r="AA34" s="89"/>
       <c r="AB34" s="11">
         <v>0.60416666666666663</v>
       </c>
@@ -2773,11 +2774,11 @@
         <v>44677</v>
       </c>
       <c r="AH34" s="5"/>
-      <c r="AI34" s="65" t="s">
+      <c r="AI34" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="AJ34" s="65"/>
-      <c r="AK34" s="65"/>
+      <c r="AJ34" s="66"/>
+      <c r="AK34" s="66"/>
       <c r="AL34" s="39">
         <v>0.70833333333333337</v>
       </c>
@@ -2789,18 +2790,18 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C35" s="30">
         <v>44638</v>
       </c>
       <c r="D35">
         <v>24</v>
       </c>
-      <c r="E35" s="66" t="s">
+      <c r="E35" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="66"/>
-      <c r="G35" s="66"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
       <c r="H35" s="11">
         <v>0.625</v>
       </c>
@@ -2836,11 +2837,11 @@
         <v>44643</v>
       </c>
       <c r="X35" s="5"/>
-      <c r="Y35" s="69" t="s">
+      <c r="Y35" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="Z35" s="69"/>
-      <c r="AA35" s="69"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="94"/>
       <c r="AB35" s="39">
         <v>0.49305555555555558</v>
       </c>
@@ -2852,15 +2853,15 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C36" s="30">
         <v>44641</v>
       </c>
-      <c r="E36" s="66" t="s">
+      <c r="E36" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
       <c r="H36" s="11">
         <v>0.625</v>
       </c>
@@ -2896,9 +2897,9 @@
       <c r="W36" s="30">
         <v>44655</v>
       </c>
-      <c r="X36" s="68"/>
-      <c r="Y36" s="68"/>
-      <c r="Z36" s="68"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
       <c r="AA36" s="11"/>
       <c r="AB36" s="11">
         <v>0.33333333333333331</v>
@@ -2911,15 +2912,15 @@
         <v>7.2916666666666685E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C37" s="30">
         <v>44646</v>
       </c>
-      <c r="E37" s="66" t="s">
+      <c r="E37" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
       <c r="H37" s="11">
         <v>0.625</v>
       </c>
@@ -2953,9 +2954,9 @@
       <c r="W37" s="30">
         <v>44655</v>
       </c>
-      <c r="X37" s="68"/>
-      <c r="Y37" s="68"/>
-      <c r="Z37" s="68"/>
+      <c r="X37" s="89"/>
+      <c r="Y37" s="89"/>
+      <c r="Z37" s="89"/>
       <c r="AA37" s="11"/>
       <c r="AB37" s="11">
         <v>0.61111111111111105</v>
@@ -2968,18 +2969,18 @@
         <v>9.7222222222222321E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="41">
         <v>44647</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="65" t="s">
+      <c r="E38" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
       <c r="H38" s="39">
         <v>0.83333333333333337</v>
       </c>
@@ -3018,11 +3019,11 @@
       <c r="W38" s="30">
         <v>44669</v>
       </c>
-      <c r="Y38" s="68" t="s">
+      <c r="Y38" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="Z38" s="68"/>
-      <c r="AA38" s="68"/>
+      <c r="Z38" s="89"/>
+      <c r="AA38" s="89"/>
       <c r="AB38" s="11">
         <v>0.58333333333333337</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="M39" s="30">
         <v>44651</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>2.569444444444452E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="M40" s="30">
         <v>44657</v>
       </c>
@@ -3076,50 +3077,26 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="M41" s="30">
+        <v>44669</v>
+      </c>
+      <c r="O41" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="R41" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="S41" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="T41" s="49">
+        <f t="shared" si="7"/>
+        <v>0.125</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="AI22:AK22"/>
-    <mergeCell ref="AI23:AK23"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="Y29:AA29"/>
-    <mergeCell ref="Y31:AA31"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="J3:L3"/>
     <mergeCell ref="AI34:AK34"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E37:G37"/>
@@ -3133,6 +3110,48 @@
     <mergeCell ref="X36:Z36"/>
     <mergeCell ref="X37:Z37"/>
     <mergeCell ref="Y38:AA38"/>
+    <mergeCell ref="Y29:AA29"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="AI22:AK22"/>
+    <mergeCell ref="AI23:AK23"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E30:G30"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added todays activities to the record
</commit_message>
<xml_diff>
--- a/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
+++ b/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Schule\SYP\Project Repo\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDAEFCC-0767-4B92-9B00-55B0406CDAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD6D797-8816-47DB-BC45-136697E356DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>Stundenaufzeichnung Sommersemester</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>ERD , md generator</t>
+  </si>
+  <si>
+    <t>working md generator</t>
   </si>
 </sst>
 </file>
@@ -918,18 +921,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -989,18 +1002,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1283,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G32" zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T63" sqref="T63"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="35" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,35 +1320,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
     </row>
     <row r="3" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="J3" s="98" t="s">
+      <c r="J3" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
@@ -1363,10 +1366,10 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="82"/>
+      <c r="F4" s="84"/>
       <c r="I4" s="11"/>
       <c r="J4" s="14"/>
       <c r="K4" s="10"/>
@@ -1379,10 +1382,10 @@
       <c r="R4" s="11"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="81"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="3">
         <v>44620</v>
       </c>
@@ -1423,10 +1426,10 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="81"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="3">
         <v>44634</v>
       </c>
@@ -1460,10 +1463,10 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="81"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="3">
         <v>44648</v>
       </c>
@@ -1497,10 +1500,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="81"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="3">
         <v>44676</v>
       </c>
@@ -1532,10 +1535,10 @@
       <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="81"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="28">
@@ -1619,11 +1622,11 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
       <c r="I12" s="11"/>
       <c r="J12" s="14">
         <v>12</v>
@@ -1675,10 +1678,10 @@
       <c r="G14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="90" t="s">
+      <c r="H14" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="91"/>
+      <c r="I14" s="93"/>
       <c r="J14" s="14">
         <v>14</v>
       </c>
@@ -1694,10 +1697,10 @@
       <c r="R14" s="22"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="85"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="17">
         <f>SUM(J23:J31)</f>
         <v>0.53819444444444442</v>
@@ -1715,11 +1718,11 @@
         <v>0.96111111111111081</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="92">
+      <c r="H15" s="94">
         <f>SUM(C15:G15)</f>
         <v>2.9972222222222218</v>
       </c>
-      <c r="I15" s="93"/>
+      <c r="I15" s="95"/>
       <c r="J15" s="14">
         <v>17</v>
       </c>
@@ -1735,10 +1738,10 @@
       <c r="R15" s="22"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="17">
         <f>SUM(T23:T29)</f>
         <v>0.44444444444444448</v>
@@ -1756,11 +1759,11 @@
         <v>1.0451388888888888</v>
       </c>
       <c r="G16" s="20"/>
-      <c r="H16" s="94">
+      <c r="H16" s="96">
         <f>SUM(C16:G16)</f>
         <v>2.9638888888888886</v>
       </c>
-      <c r="I16" s="95"/>
+      <c r="I16" s="97"/>
       <c r="J16" s="14">
         <v>44</v>
       </c>
@@ -1781,10 +1784,10 @@
       <c r="R16" s="22"/>
     </row>
     <row r="17" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="89"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="18">
         <f>SUM(AD23:AD28)</f>
         <v>0.4472222222222223</v>
@@ -1802,11 +1805,11 @@
         <v>0.88888888888888906</v>
       </c>
       <c r="G17" s="19"/>
-      <c r="H17" s="96">
+      <c r="H17" s="98">
         <f>SUM(C17:G17)</f>
         <v>2.5756944444444452</v>
       </c>
-      <c r="I17" s="97"/>
+      <c r="I17" s="99"/>
       <c r="J17" s="14">
         <v>22</v>
       </c>
@@ -1839,8 +1842,8 @@
     </row>
     <row r="19" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="85"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
@@ -1855,11 +1858,11 @@
       <c r="D22" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="77" t="s">
+      <c r="E22" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
       <c r="H22" s="33" t="s">
         <v>21</v>
       </c>
@@ -1879,11 +1882,11 @@
       <c r="N22" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="O22" s="77" t="s">
+      <c r="O22" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77"/>
+      <c r="P22" s="76"/>
+      <c r="Q22" s="76"/>
       <c r="R22" s="33" t="s">
         <v>21</v>
       </c>
@@ -1903,11 +1906,11 @@
       <c r="X22" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="Y22" s="77" t="s">
+      <c r="Y22" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="Z22" s="77"/>
-      <c r="AA22" s="77"/>
+      <c r="Z22" s="76"/>
+      <c r="AA22" s="76"/>
       <c r="AB22" s="33" t="s">
         <v>21</v>
       </c>
@@ -1929,11 +1932,11 @@
         <v>44622</v>
       </c>
       <c r="D23" s="32"/>
-      <c r="E23" s="78" t="s">
+      <c r="E23" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="H23" s="42">
         <v>0.49305555555555558</v>
       </c>
@@ -2390,11 +2393,11 @@
         <v>44634</v>
       </c>
       <c r="X29" s="32"/>
-      <c r="Y29" s="78" t="s">
+      <c r="Y29" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="Z29" s="78"/>
-      <c r="AA29" s="78"/>
+      <c r="Z29" s="73"/>
+      <c r="AA29" s="73"/>
       <c r="AB29" s="55">
         <v>0.64583333333333337</v>
       </c>
@@ -2461,11 +2464,11 @@
         <v>44635</v>
       </c>
       <c r="X30" s="31"/>
-      <c r="Y30" s="100" t="s">
+      <c r="Y30" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="Z30" s="100"/>
-      <c r="AA30" s="100"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="78"/>
       <c r="AB30" s="55">
         <v>0.625</v>
       </c>
@@ -2486,11 +2489,11 @@
       <c r="D31" s="33">
         <v>44.46</v>
       </c>
-      <c r="E31" s="77" t="s">
+      <c r="E31" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
       <c r="H31" s="50">
         <v>0.8125</v>
       </c>
@@ -2530,11 +2533,11 @@
         <v>44637</v>
       </c>
       <c r="X31" s="31"/>
-      <c r="Y31" s="100" t="s">
+      <c r="Y31" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="Z31" s="100"/>
-      <c r="AA31" s="100"/>
+      <c r="Z31" s="78"/>
+      <c r="AA31" s="78"/>
       <c r="AB31" s="55">
         <v>0.83333333333333337</v>
       </c>
@@ -2559,11 +2562,11 @@
       <c r="D32" s="56">
         <v>46</v>
       </c>
-      <c r="E32" s="78" t="s">
+      <c r="E32" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
       <c r="H32" s="42">
         <v>0.64583333333333337</v>
       </c>
@@ -2810,11 +2813,11 @@
         <v>44643</v>
       </c>
       <c r="X35" s="33"/>
-      <c r="Y35" s="77" t="s">
+      <c r="Y35" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="Z35" s="77"/>
-      <c r="AA35" s="77"/>
+      <c r="Z35" s="76"/>
+      <c r="AA35" s="76"/>
       <c r="AB35" s="50">
         <v>0.49305555555555558</v>
       </c>
@@ -2879,11 +2882,11 @@
         <v>44655</v>
       </c>
       <c r="X36" s="32"/>
-      <c r="Y36" s="78" t="s">
+      <c r="Y36" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="Z36" s="78"/>
-      <c r="AA36" s="78"/>
+      <c r="Z36" s="73"/>
+      <c r="AA36" s="73"/>
       <c r="AB36" s="42">
         <v>0.33333333333333331</v>
       </c>
@@ -2969,11 +2972,11 @@
         <v>44647</v>
       </c>
       <c r="D38" s="33"/>
-      <c r="E38" s="77" t="s">
+      <c r="E38" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="50">
         <v>0.83333333333333337</v>
       </c>
@@ -3040,11 +3043,11 @@
         <v>44651</v>
       </c>
       <c r="D39" s="32"/>
-      <c r="E39" s="78" t="s">
+      <c r="E39" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
       <c r="H39" s="66">
         <v>0.35416666666666669</v>
       </c>
@@ -3197,11 +3200,11 @@
       <c r="N41" s="56">
         <v>46</v>
       </c>
-      <c r="O41" s="76" t="s">
+      <c r="O41" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="P41" s="76"/>
-      <c r="Q41" s="76"/>
+      <c r="P41" s="75"/>
+      <c r="Q41" s="75"/>
       <c r="R41" s="42">
         <v>0.65</v>
       </c>
@@ -3350,11 +3353,11 @@
         <v>44669</v>
       </c>
       <c r="X43" s="33"/>
-      <c r="Y43" s="77" t="s">
+      <c r="Y43" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="Z43" s="77"/>
-      <c r="AA43" s="77"/>
+      <c r="Z43" s="76"/>
+      <c r="AA43" s="76"/>
       <c r="AB43" s="50">
         <v>0.58333333333333337</v>
       </c>
@@ -3419,11 +3422,11 @@
         <v>44676</v>
       </c>
       <c r="X44" s="34"/>
-      <c r="Y44" s="78" t="s">
+      <c r="Y44" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="Z44" s="78"/>
-      <c r="AA44" s="78"/>
+      <c r="Z44" s="73"/>
+      <c r="AA44" s="73"/>
       <c r="AB44" s="61">
         <v>0.75</v>
       </c>
@@ -3465,11 +3468,11 @@
       <c r="N45" s="56">
         <v>7</v>
       </c>
-      <c r="O45" s="76" t="s">
+      <c r="O45" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="P45" s="76"/>
-      <c r="Q45" s="76"/>
+      <c r="P45" s="75"/>
+      <c r="Q45" s="75"/>
       <c r="R45" s="42">
         <v>0.58333333333333337</v>
       </c>
@@ -3486,11 +3489,11 @@
         <v>44676</v>
       </c>
       <c r="X45" s="32"/>
-      <c r="Y45" s="78" t="s">
+      <c r="Y45" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="Z45" s="78"/>
-      <c r="AA45" s="78"/>
+      <c r="Z45" s="73"/>
+      <c r="AA45" s="73"/>
       <c r="AB45" s="42">
         <v>0.61111111111111105</v>
       </c>
@@ -3509,11 +3512,11 @@
         <v>44667</v>
       </c>
       <c r="D46" s="33"/>
-      <c r="E46" s="77" t="s">
+      <c r="E46" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="77"/>
-      <c r="G46" s="77"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
       <c r="H46" s="50">
         <v>0.39097222222222222</v>
       </c>
@@ -3532,11 +3535,11 @@
       <c r="N46" s="56">
         <v>7</v>
       </c>
-      <c r="O46" s="76" t="s">
+      <c r="O46" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="P46" s="76"/>
-      <c r="Q46" s="76"/>
+      <c r="P46" s="75"/>
+      <c r="Q46" s="75"/>
       <c r="R46" s="42">
         <v>0.70833333333333337</v>
       </c>
@@ -3601,11 +3604,11 @@
       <c r="N47" s="67">
         <v>7</v>
       </c>
-      <c r="O47" s="101" t="s">
+      <c r="O47" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="P47" s="101"/>
-      <c r="Q47" s="101"/>
+      <c r="P47" s="77"/>
+      <c r="Q47" s="77"/>
       <c r="R47" s="50">
         <v>0.9375</v>
       </c>
@@ -3668,11 +3671,11 @@
       <c r="N48" s="36">
         <v>42</v>
       </c>
-      <c r="O48" s="78" t="s">
+      <c r="O48" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
+      <c r="P48" s="73"/>
+      <c r="Q48" s="73"/>
       <c r="R48" s="42">
         <v>0.66666666666666663</v>
       </c>
@@ -4382,9 +4385,9 @@
       <c r="L60" s="70"/>
       <c r="M60" s="70"/>
       <c r="N60" s="70"/>
-      <c r="O60" s="75"/>
-      <c r="P60" s="75"/>
-      <c r="Q60" s="75"/>
+      <c r="O60" s="101"/>
+      <c r="P60" s="101"/>
+      <c r="Q60" s="101"/>
       <c r="R60" s="70"/>
       <c r="S60" s="70"/>
       <c r="T60" s="70"/>
@@ -4409,11 +4412,11 @@
       <c r="M61" s="71">
         <v>44705</v>
       </c>
-      <c r="O61" s="76" t="s">
+      <c r="O61" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="P61" s="76"/>
-      <c r="Q61" s="76"/>
+      <c r="P61" s="75"/>
+      <c r="Q61" s="75"/>
       <c r="R61" s="72">
         <v>0.70833333333333337</v>
       </c>
@@ -4440,11 +4443,11 @@
       <c r="M62" s="71">
         <v>44706</v>
       </c>
-      <c r="O62" s="76" t="s">
+      <c r="O62" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="P62" s="76"/>
-      <c r="Q62" s="76"/>
+      <c r="P62" s="75"/>
+      <c r="Q62" s="75"/>
       <c r="R62" s="72">
         <v>0.48958333333333331</v>
       </c>
@@ -4457,32 +4460,137 @@
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="O63" s="73"/>
-      <c r="P63" s="73"/>
-      <c r="Q63" s="73"/>
+      <c r="M63" s="71">
+        <v>44678</v>
+      </c>
+      <c r="O63" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="P63" s="75"/>
+      <c r="Q63" s="75"/>
+      <c r="R63" s="72">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="S63" s="72">
+        <v>0.83124999999999993</v>
+      </c>
+      <c r="T63" s="72">
+        <f>SUM(S63-R63)</f>
+        <v>0.18541666666666656</v>
+      </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="O64" s="73"/>
-      <c r="P64" s="73"/>
-      <c r="Q64" s="73"/>
+      <c r="O64" s="100"/>
+      <c r="P64" s="100"/>
+      <c r="Q64" s="100"/>
     </row>
     <row r="65" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O65" s="73"/>
-      <c r="P65" s="73"/>
-      <c r="Q65" s="73"/>
+      <c r="O65" s="100"/>
+      <c r="P65" s="100"/>
+      <c r="Q65" s="100"/>
     </row>
     <row r="66" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O66" s="73"/>
-      <c r="P66" s="73"/>
-      <c r="Q66" s="73"/>
+      <c r="O66" s="100"/>
+      <c r="P66" s="100"/>
+      <c r="Q66" s="100"/>
     </row>
     <row r="67" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O67" s="73"/>
-      <c r="P67" s="73"/>
-      <c r="Q67" s="73"/>
+      <c r="O67" s="100"/>
+      <c r="P67" s="100"/>
+      <c r="Q67" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="O64:Q64"/>
+    <mergeCell ref="O65:Q65"/>
+    <mergeCell ref="O66:Q66"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="Y51:AA51"/>
+    <mergeCell ref="O59:Q59"/>
+    <mergeCell ref="O60:Q60"/>
+    <mergeCell ref="O61:Q61"/>
+    <mergeCell ref="O62:Q62"/>
+    <mergeCell ref="O63:Q63"/>
+    <mergeCell ref="O54:Q54"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="O57:Q57"/>
+    <mergeCell ref="O58:Q58"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="Y40:AA40"/>
+    <mergeCell ref="Y41:AA41"/>
+    <mergeCell ref="Y42:AA42"/>
+    <mergeCell ref="Y29:AA29"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="Y39:AA39"/>
+    <mergeCell ref="Y30:AA30"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="Y33:AA33"/>
+    <mergeCell ref="Y34:AA34"/>
+    <mergeCell ref="Y35:AA35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="Y38:AA38"/>
+    <mergeCell ref="Y36:AA36"/>
+    <mergeCell ref="Y37:AA37"/>
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="Y45:AA45"/>
     <mergeCell ref="Y46:AA46"/>
@@ -4505,96 +4613,6 @@
     <mergeCell ref="O51:Q51"/>
     <mergeCell ref="O52:Q52"/>
     <mergeCell ref="O53:Q53"/>
-    <mergeCell ref="Y40:AA40"/>
-    <mergeCell ref="Y41:AA41"/>
-    <mergeCell ref="Y42:AA42"/>
-    <mergeCell ref="Y29:AA29"/>
-    <mergeCell ref="Y31:AA31"/>
-    <mergeCell ref="Y39:AA39"/>
-    <mergeCell ref="Y30:AA30"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="Y33:AA33"/>
-    <mergeCell ref="Y34:AA34"/>
-    <mergeCell ref="Y35:AA35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="Y38:AA38"/>
-    <mergeCell ref="Y36:AA36"/>
-    <mergeCell ref="Y37:AA37"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="O64:Q64"/>
-    <mergeCell ref="O65:Q65"/>
-    <mergeCell ref="O66:Q66"/>
-    <mergeCell ref="O67:Q67"/>
-    <mergeCell ref="Y51:AA51"/>
-    <mergeCell ref="O59:Q59"/>
-    <mergeCell ref="O60:Q60"/>
-    <mergeCell ref="O61:Q61"/>
-    <mergeCell ref="O62:Q62"/>
-    <mergeCell ref="O63:Q63"/>
-    <mergeCell ref="O54:Q54"/>
-    <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="O56:Q56"/>
-    <mergeCell ref="O57:Q57"/>
-    <mergeCell ref="O58:Q58"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed layout of Stundenaufzeichnung
</commit_message>
<xml_diff>
--- a/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
+++ b/Dokumente/Sundenauzeichnung_Sommersemester.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimne/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Schule\SYP\Project Repo\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6998C53B-6A6B-A94B-8508-9DCC22384DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA197E78-B1AD-4059-8B1D-50B318D27D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stundenaufzeichnung" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -544,7 +542,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -760,22 +758,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -952,25 +939,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -988,9 +994,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1027,18 +1030,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1319,65 +1319,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD71"/>
+  <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="137" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC66" sqref="AC66"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="33" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="W83" sqref="W83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6328125" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.1640625" customWidth="1"/>
-    <col min="22" max="22" width="18.83203125" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.36328125" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" customWidth="1"/>
+    <col min="22" max="22" width="18.81640625" customWidth="1"/>
+    <col min="23" max="23" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-    </row>
-    <row r="2" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
       <c r="J2" s="49"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1389,14 +1389,14 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I3" s="76"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
       <c r="P3" s="42"/>
@@ -1404,7 +1404,7 @@
       <c r="R3" s="42"/>
       <c r="S3" s="43"/>
     </row>
-    <row r="4" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1414,10 +1414,10 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="92"/>
+      <c r="F4" s="97"/>
       <c r="I4" s="5"/>
       <c r="J4" s="53"/>
       <c r="K4" s="41"/>
@@ -1430,11 +1430,11 @@
       <c r="R4" s="42"/>
       <c r="S4" s="43"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="91" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="91"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="3">
         <v>44620</v>
       </c>
@@ -1475,11 +1475,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="91" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="91"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="3">
         <v>44634</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="P6" s="47">
-        <f>J36</f>
+        <f>J35</f>
         <v>0.10416666666666663</v>
       </c>
       <c r="Q6" s="5">
@@ -1513,11 +1513,11 @@
       <c r="R6" s="5"/>
       <c r="S6" s="46"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="91"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="3">
         <v>44648</v>
       </c>
@@ -1547,15 +1547,15 @@
         <v>4</v>
       </c>
       <c r="S7" s="47">
-        <f>SUM(J54,J57,J58,J61,T50,T51,T52,AD56)</f>
+        <f>SUM(J53,J56,J57,J60,T50,T51,T52,AD56)</f>
         <v>0.61111111111111105</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="91"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="3">
         <v>44676</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="47">
-        <f>J35</f>
+        <f>J34</f>
         <v>9.9305555555555536E-2</v>
       </c>
       <c r="Q8" s="5">
@@ -1587,11 +1587,11 @@
       <c r="R8" s="5"/>
       <c r="S8" s="47"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="91" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="9">
@@ -1622,7 +1622,7 @@
         <v>4.513888888888884E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I10" s="5"/>
       <c r="J10" s="53"/>
       <c r="K10" s="5">
@@ -1642,11 +1642,11 @@
         <v>72</v>
       </c>
       <c r="S10" s="47">
-        <f>J29+J30+T26+T32+AD35+T35+T36+T37+T38+T39+T41+T40+T42+T43+T33</f>
+        <f>J28+J29+T26+T32+AD35+T35+T36+T37+T38+T39+T41+T40+T42+T43+T33</f>
         <v>1.0979166666666669</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -1674,11 +1674,11 @@
         <v>1.2</v>
       </c>
       <c r="S11" s="47">
-        <f>J26+J27+J28+J31+T29+T26+T25+T24+AD28</f>
+        <f>J25+J26+J27+J30+T29+T26+T25+T24+AD28</f>
         <v>0.62083333333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="49"/>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
@@ -1710,12 +1710,12 @@
         <v>0.66388888888888886</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
       <c r="I13" s="5"/>
       <c r="J13" s="44"/>
       <c r="K13" s="5">
@@ -1739,7 +1739,7 @@
         <v>0.66388888888888886</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I14" s="5"/>
       <c r="J14" s="53"/>
       <c r="K14" s="5">
@@ -1756,7 +1756,7 @@
       <c r="R14" s="5"/>
       <c r="S14" s="47"/>
     </row>
-    <row r="15" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="55" t="s">
         <v>2</v>
       </c>
@@ -1776,10 +1776,10 @@
       <c r="G15" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="100" t="s">
+      <c r="H15" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="I15" s="100"/>
+      <c r="I15" s="104"/>
       <c r="J15" s="78" t="s">
         <v>14</v>
       </c>
@@ -1797,33 +1797,33 @@
       <c r="R15" s="5"/>
       <c r="S15" s="47"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="95" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="96"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="6">
-        <f>SUM(J24:J32)</f>
+        <f>SUM(J23:J31)</f>
         <v>0.53819444444444442</v>
       </c>
       <c r="D16" s="6">
-        <f>SUM(J33:J39)</f>
+        <f>SUM(J32:J38)</f>
         <v>0.55069444444444438</v>
       </c>
       <c r="E16" s="6">
-        <f>SUM(J41:J48)</f>
+        <f>SUM(J40:J47)</f>
         <v>0.94722222222222219</v>
       </c>
       <c r="F16" s="6">
-        <f>SUM(J51:J69)</f>
+        <f>SUM(J50:J69)</f>
         <v>1.5506944444444444</v>
       </c>
       <c r="G16" s="6">
         <f>SUM(J64:J73)</f>
         <v>0.58958333333333346</v>
       </c>
-      <c r="H16" s="101"/>
-      <c r="I16" s="102"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="106"/>
       <c r="J16" s="54">
         <f>SUM(C16:F16)</f>
         <v>3.5868055555555554</v>
@@ -1835,7 +1835,7 @@
         <v>1.2</v>
       </c>
       <c r="M16" s="47">
-        <f>J26+J27+J28+J29+T24+T25+T26+T29+AD28+AD35</f>
+        <f>J25+J26+J27+J28+T24+T25+T26+T29+AD28+AD35</f>
         <v>0.68333333333333335</v>
       </c>
       <c r="N16" s="5">
@@ -1847,11 +1847,11 @@
       <c r="R16" s="5"/>
       <c r="S16" s="47"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A17" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="96"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="6">
         <f>SUM(T23:T29)</f>
         <v>0.44444444444444448</v>
@@ -1872,8 +1872,8 @@
         <f>SUM(T64:T67:T68,T69)</f>
         <v>0.66388888888888886</v>
       </c>
-      <c r="H17" s="103"/>
-      <c r="I17" s="104"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="108"/>
       <c r="J17" s="54">
         <f>SUM(C17:G17)</f>
         <v>3.6277777777777773</v>
@@ -1892,11 +1892,11 @@
       <c r="R17" s="5"/>
       <c r="S17" s="47"/>
     </row>
-    <row r="18" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+    <row r="18" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="99"/>
+      <c r="B18" s="103"/>
       <c r="C18" s="58">
         <f>SUM(AD23:AD28)</f>
         <v>0.4472222222222223</v>
@@ -1917,8 +1917,8 @@
         <f>SUM(AD64:AD68)</f>
         <v>0.63125000000000009</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="110"/>
       <c r="J18" s="77">
         <f>SUM(C18:F18)</f>
         <v>2.5756944444444452</v>
@@ -1937,17 +1937,41 @@
       <c r="R18" s="49"/>
       <c r="S18" s="51"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="H19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="76"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="J20" s="5"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="93"/>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="K22" s="13" t="s">
         <v>2</v>
       </c>
@@ -1958,11 +1982,11 @@
       <c r="N22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O22" s="94" t="s">
+      <c r="O22" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
+      <c r="P22" s="89"/>
+      <c r="Q22" s="89"/>
       <c r="R22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1982,11 +2006,11 @@
       <c r="X22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Y22" s="94" t="s">
+      <c r="Y22" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="Z22" s="94"/>
-      <c r="AA22" s="94"/>
+      <c r="Z22" s="89"/>
+      <c r="AA22" s="89"/>
       <c r="AB22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1997,32 +2021,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="94" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>23</v>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="20">
+        <v>44622</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="21">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="I23" s="21">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="J23" s="22">
+        <f t="shared" ref="J23:J64" si="0">I23-H23</f>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>4</v>
@@ -2034,11 +2057,11 @@
         <v>44626</v>
       </c>
       <c r="N23" s="24"/>
-      <c r="O23" s="85" t="s">
+      <c r="O23" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="P23" s="85"/>
-      <c r="Q23" s="85"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="86"/>
       <c r="R23" s="21">
         <v>0.79166666666666663</v>
       </c>
@@ -2059,11 +2082,11 @@
         <v>44626</v>
       </c>
       <c r="X23" s="12"/>
-      <c r="Y23" s="85" t="s">
+      <c r="Y23" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="Z23" s="85"/>
-      <c r="AA23" s="85"/>
+      <c r="Z23" s="86"/>
+      <c r="AA23" s="86"/>
       <c r="AB23" s="21">
         <v>0.79166666666666663</v>
       </c>
@@ -2075,31 +2098,27 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>7</v>
-      </c>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="20">
-        <v>44622</v>
+        <v>44626</v>
       </c>
       <c r="D24" s="12"/>
-      <c r="E24" s="109" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
+      <c r="E24" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
       <c r="H24" s="21">
-        <v>0.49305555555555558</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="I24" s="21">
-        <v>0.52777777777777779</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="J24" s="22">
-        <f t="shared" ref="J24:J64" si="0">I24-H24</f>
-        <v>3.472222222222221E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -2146,27 +2165,27 @@
         <v>7.2916666666666741E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="20">
-        <v>44626</v>
+        <v>44627</v>
       </c>
       <c r="D25" s="12"/>
-      <c r="E25" s="85" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
+      <c r="E25" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
       <c r="H25" s="21">
-        <v>0.79166666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I25" s="21">
-        <v>0.85416666666666663</v>
+        <v>0.40625</v>
       </c>
       <c r="J25" s="22">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>7.2916666666666685E-2</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2197,10 +2216,10 @@
         <v>44630</v>
       </c>
       <c r="X25" s="12"/>
-      <c r="Y25" s="85" t="s">
+      <c r="Y25" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="Z25" s="85"/>
+      <c r="Z25" s="86"/>
       <c r="AA25" s="12"/>
       <c r="AB25" s="21">
         <v>0.75</v>
@@ -2213,27 +2232,27 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="20">
         <v>44627</v>
       </c>
       <c r="D26" s="12"/>
-      <c r="E26" s="85" t="s">
+      <c r="E26" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="H26" s="21">
-        <v>0.33333333333333331</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I26" s="21">
-        <v>0.40625</v>
+        <v>0.875</v>
       </c>
       <c r="J26" s="22">
         <f t="shared" si="0"/>
-        <v>7.2916666666666685E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -2264,11 +2283,11 @@
         <v>44630</v>
       </c>
       <c r="X26" s="12"/>
-      <c r="Y26" s="85" t="s">
+      <c r="Y26" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="Z26" s="85"/>
-      <c r="AA26" s="85"/>
+      <c r="Z26" s="86"/>
+      <c r="AA26" s="86"/>
       <c r="AB26" s="21">
         <v>0.875</v>
       </c>
@@ -2280,27 +2299,29 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="20">
-        <v>44627</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
+        <v>44629</v>
+      </c>
+      <c r="D27" s="12">
+        <v>44.47</v>
+      </c>
+      <c r="E27" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="H27" s="21">
-        <v>0.83333333333333337</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="I27" s="21">
-        <v>0.875</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="J27" s="22">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
@@ -2310,11 +2331,11 @@
       <c r="N27" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O27" s="85" t="s">
+      <c r="O27" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="P27" s="85"/>
-      <c r="Q27" s="85"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="86"/>
       <c r="R27" s="21">
         <v>0.76041666666666663</v>
       </c>
@@ -2347,7 +2368,7 @@
         <v>6.8055555555555536E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="20">
@@ -2356,20 +2377,20 @@
       <c r="D28" s="12">
         <v>44.47</v>
       </c>
-      <c r="E28" s="85" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
+      <c r="E28" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
       <c r="H28" s="21">
-        <v>0.49305555555555558</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="I28" s="21">
-        <v>0.52777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J28" s="22">
         <f t="shared" si="0"/>
-        <v>3.472222222222221E-2</v>
+        <v>0.10416666666666674</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
@@ -2417,29 +2438,29 @@
         <v>5.6250000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="20">
-        <v>44629</v>
+        <v>44630</v>
       </c>
       <c r="D29" s="12">
         <v>44.47</v>
       </c>
-      <c r="E29" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
+      <c r="E29" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
       <c r="H29" s="21">
-        <v>0.72916666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="I29" s="21">
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J29" s="22">
         <f t="shared" si="0"/>
-        <v>0.10416666666666674</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="K29" s="61"/>
       <c r="L29" s="39"/>
@@ -2475,29 +2496,29 @@
       <c r="AC29" s="29"/>
       <c r="AD29" s="22"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="20">
-        <v>44630</v>
+        <v>44631</v>
       </c>
       <c r="D30" s="12">
         <v>44.47</v>
       </c>
-      <c r="E30" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85"/>
+      <c r="E30" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
       <c r="H30" s="21">
         <v>0.625</v>
       </c>
       <c r="I30" s="21">
-        <v>0.66666666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="J30" s="22">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="K30" s="39"/>
       <c r="L30" s="39"/>
@@ -2520,29 +2541,29 @@
       <c r="AC30" s="29"/>
       <c r="AD30" s="22"/>
     </row>
-    <row r="31" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="20">
-        <v>44631</v>
-      </c>
-      <c r="D31" s="12">
-        <v>44.47</v>
-      </c>
-      <c r="E31" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="21">
-        <v>0.625</v>
-      </c>
-      <c r="I31" s="21">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="J31" s="22">
+    <row r="31" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="66"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="67">
+        <v>44633</v>
+      </c>
+      <c r="D31" s="66">
+        <v>44.46</v>
+      </c>
+      <c r="E31" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="64">
+        <v>0.8125</v>
+      </c>
+      <c r="I31" s="64">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="J31" s="65">
         <f t="shared" si="0"/>
-        <v>0.10416666666666663</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="K31" s="66"/>
       <c r="L31" s="66"/>
@@ -2565,29 +2586,33 @@
       <c r="AC31" s="64"/>
       <c r="AD31" s="70"/>
     </row>
-    <row r="32" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="67">
-        <v>44633</v>
-      </c>
-      <c r="D32" s="66">
-        <v>44.46</v>
-      </c>
-      <c r="E32" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="64">
-        <v>0.8125</v>
-      </c>
-      <c r="I32" s="64">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="J32" s="65">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="20">
+        <v>44634</v>
+      </c>
+      <c r="D32" s="30">
+        <v>46</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I32" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="J32" s="31">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="14" t="s">
@@ -2622,11 +2647,11 @@
         <v>44634</v>
       </c>
       <c r="X32" s="12"/>
-      <c r="Y32" s="88" t="s">
+      <c r="Y32" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="Z32" s="88"/>
-      <c r="AA32" s="88"/>
+      <c r="Z32" s="85"/>
+      <c r="AA32" s="85"/>
       <c r="AB32" s="29">
         <v>0.64583333333333337</v>
       </c>
@@ -2638,33 +2663,29 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>8</v>
-      </c>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="20">
-        <v>44634</v>
-      </c>
-      <c r="D33" s="30">
-        <v>46</v>
-      </c>
-      <c r="E33" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="88"/>
+        <v>44636</v>
+      </c>
+      <c r="D33" s="12">
+        <v>47</v>
+      </c>
+      <c r="E33" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
       <c r="H33" s="21">
-        <v>0.64583333333333337</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="I33" s="21">
-        <v>0.70833333333333337</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="J33" s="31">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
@@ -2695,11 +2716,11 @@
         <v>44635</v>
       </c>
       <c r="X33" s="11"/>
-      <c r="Y33" s="88" t="s">
+      <c r="Y33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="Z33" s="88"/>
-      <c r="AA33" s="88"/>
+      <c r="Z33" s="85"/>
+      <c r="AA33" s="85"/>
       <c r="AB33" s="29">
         <v>0.625</v>
       </c>
@@ -2711,29 +2732,29 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="20">
-        <v>44636</v>
+        <v>44637</v>
       </c>
       <c r="D34" s="12">
-        <v>47</v>
-      </c>
-      <c r="E34" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
+        <v>26</v>
+      </c>
+      <c r="E34" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
       <c r="H34" s="21">
-        <v>0.49305555555555558</v>
+        <v>0.75</v>
       </c>
       <c r="I34" s="21">
-        <v>0.52777777777777779</v>
+        <v>0.84930555555555554</v>
       </c>
       <c r="J34" s="31">
         <f t="shared" si="0"/>
-        <v>3.472222222222221E-2</v>
+        <v>9.9305555555555536E-2</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -2762,11 +2783,11 @@
         <v>44637</v>
       </c>
       <c r="X34" s="11"/>
-      <c r="Y34" s="88" t="s">
+      <c r="Y34" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="Z34" s="88"/>
-      <c r="AA34" s="88"/>
+      <c r="Z34" s="85"/>
+      <c r="AA34" s="85"/>
       <c r="AB34" s="29">
         <v>0.83333333333333337</v>
       </c>
@@ -2778,29 +2799,29 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="20">
-        <v>44637</v>
+        <v>44638</v>
       </c>
       <c r="D35" s="12">
-        <v>26</v>
-      </c>
-      <c r="E35" s="85" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
+        <v>24</v>
+      </c>
+      <c r="E35" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="21">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="I35" s="21">
-        <v>0.84930555555555554</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="J35" s="31">
         <f t="shared" si="0"/>
-        <v>9.9305555555555536E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
@@ -2849,29 +2870,27 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="20">
-        <v>44638</v>
-      </c>
-      <c r="D36" s="12">
-        <v>24</v>
-      </c>
-      <c r="E36" s="85" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="85"/>
-      <c r="G36" s="85"/>
+        <v>44641</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="86" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
       <c r="H36" s="21">
         <v>0.625</v>
       </c>
       <c r="I36" s="21">
-        <v>0.72916666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="J36" s="31">
         <f t="shared" si="0"/>
-        <v>0.10416666666666663</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
@@ -2902,11 +2921,11 @@
         <v>44641</v>
       </c>
       <c r="X36" s="12"/>
-      <c r="Y36" s="85" t="s">
+      <c r="Y36" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="Z36" s="85"/>
-      <c r="AA36" s="85"/>
+      <c r="Z36" s="86"/>
+      <c r="AA36" s="86"/>
       <c r="AB36" s="21">
         <v>0.33333333333333331</v>
       </c>
@@ -2918,18 +2937,18 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="20">
-        <v>44641</v>
+        <v>44646</v>
       </c>
       <c r="D37" s="12"/>
-      <c r="E37" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
+      <c r="E37" s="86" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
       <c r="H37" s="21">
         <v>0.625</v>
       </c>
@@ -2969,11 +2988,11 @@
         <v>44642</v>
       </c>
       <c r="X37" s="12"/>
-      <c r="Y37" s="85" t="s">
+      <c r="Y37" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="Z37" s="85"/>
-      <c r="AA37" s="85"/>
+      <c r="Z37" s="86"/>
+      <c r="AA37" s="86"/>
       <c r="AB37" s="21">
         <v>0.60416666666666663</v>
       </c>
@@ -2985,27 +3004,27 @@
         <v>0.11458333333333337</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="20">
-        <v>44646</v>
-      </c>
-      <c r="D38" s="12"/>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="32">
+        <v>44647</v>
+      </c>
+      <c r="D38" s="39"/>
       <c r="E38" s="85" t="s">
         <v>68</v>
       </c>
       <c r="F38" s="85"/>
       <c r="G38" s="85"/>
-      <c r="H38" s="21">
-        <v>0.625</v>
-      </c>
-      <c r="I38" s="21">
-        <v>0.70833333333333337</v>
+      <c r="H38" s="29">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I38" s="29">
+        <v>0.91666666666666663</v>
       </c>
       <c r="J38" s="31">
         <f t="shared" si="0"/>
-        <v>8.333333333333337E-2</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
@@ -3036,11 +3055,11 @@
         <v>44643</v>
       </c>
       <c r="X38" s="39"/>
-      <c r="Y38" s="88" t="s">
+      <c r="Y38" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="Z38" s="88"/>
-      <c r="AA38" s="88"/>
+      <c r="Z38" s="85"/>
+      <c r="AA38" s="85"/>
       <c r="AB38" s="29">
         <v>0.49305555555555558</v>
       </c>
@@ -3052,28 +3071,17 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="32">
-        <v>44647</v>
-      </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="88"/>
-      <c r="H39" s="29">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="I39" s="29">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="J39" s="31">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333259E-2</v>
-      </c>
+    <row r="39" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="65"/>
       <c r="K39" s="66"/>
       <c r="L39" s="66"/>
       <c r="M39" s="67">
@@ -3108,17 +3116,30 @@
       <c r="AC39" s="64"/>
       <c r="AD39" s="65"/>
     </row>
-    <row r="40" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="66"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="65"/>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="20">
+        <v>44651</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="29">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I40" s="21">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="J40" s="31">
+        <f t="shared" si="0"/>
+        <v>0.18402777777777773</v>
+      </c>
       <c r="K40" s="71"/>
       <c r="L40" s="28" t="s">
         <v>9</v>
@@ -3152,11 +3173,11 @@
         <v>44655</v>
       </c>
       <c r="X40" s="39"/>
-      <c r="Y40" s="88" t="s">
+      <c r="Y40" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="Z40" s="88"/>
-      <c r="AA40" s="88"/>
+      <c r="Z40" s="85"/>
+      <c r="AA40" s="85"/>
       <c r="AB40" s="29">
         <v>0.33333333333333331</v>
       </c>
@@ -3168,29 +3189,27 @@
         <v>7.2916666666666685E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
-      <c r="B41" s="28" t="s">
-        <v>9</v>
-      </c>
+      <c r="B41" s="12"/>
       <c r="C41" s="20">
         <v>44651</v>
       </c>
       <c r="D41" s="12"/>
-      <c r="E41" s="88" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="88"/>
-      <c r="G41" s="88"/>
-      <c r="H41" s="29">
-        <v>0.35416666666666669</v>
+      <c r="E41" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="21">
+        <v>0.76736111111111116</v>
       </c>
       <c r="I41" s="21">
-        <v>0.53819444444444442</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="J41" s="31">
         <f t="shared" si="0"/>
-        <v>0.18402777777777773</v>
+        <v>8.6805555555555469E-2</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
@@ -3221,11 +3240,11 @@
         <v>44655</v>
       </c>
       <c r="X41" s="12"/>
-      <c r="Y41" s="85" t="s">
+      <c r="Y41" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="Z41" s="85"/>
-      <c r="AA41" s="85"/>
+      <c r="Z41" s="86"/>
+      <c r="AA41" s="86"/>
       <c r="AB41" s="21">
         <v>0.61111111111111105</v>
       </c>
@@ -3237,27 +3256,27 @@
         <v>9.7222222222222321E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="20">
-        <v>44651</v>
+        <v>44656</v>
       </c>
       <c r="D42" s="12"/>
-      <c r="E42" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
+      <c r="E42" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
       <c r="H42" s="21">
-        <v>0.76736111111111116</v>
+        <v>0.625</v>
       </c>
       <c r="I42" s="21">
-        <v>0.85416666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="J42" s="31">
         <f t="shared" si="0"/>
-        <v>8.6805555555555469E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
@@ -3288,11 +3307,11 @@
         <v>44664</v>
       </c>
       <c r="X42" s="12"/>
-      <c r="Y42" s="85" t="s">
+      <c r="Y42" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="Z42" s="85"/>
-      <c r="AA42" s="85"/>
+      <c r="Z42" s="86"/>
+      <c r="AA42" s="86"/>
       <c r="AB42" s="21">
         <v>0.875</v>
       </c>
@@ -3304,27 +3323,27 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="20">
-        <v>44656</v>
+        <v>44657</v>
       </c>
       <c r="D43" s="12"/>
-      <c r="E43" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
+      <c r="E43" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="86"/>
+      <c r="G43" s="86"/>
       <c r="H43" s="21">
-        <v>0.625</v>
+        <v>0.375</v>
       </c>
       <c r="I43" s="21">
-        <v>0.72916666666666663</v>
+        <v>0.51527777777777783</v>
       </c>
       <c r="J43" s="31">
         <f t="shared" si="0"/>
-        <v>0.10416666666666663</v>
+        <v>0.14027777777777783</v>
       </c>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
@@ -3334,11 +3353,11 @@
       <c r="N43" s="30">
         <v>46</v>
       </c>
-      <c r="O43" s="83" t="s">
+      <c r="O43" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="P43" s="83"/>
-      <c r="Q43" s="83"/>
+      <c r="P43" s="87"/>
+      <c r="Q43" s="87"/>
       <c r="R43" s="21">
         <v>0.65</v>
       </c>
@@ -3355,11 +3374,11 @@
         <v>44665</v>
       </c>
       <c r="X43" s="12"/>
-      <c r="Y43" s="85" t="s">
+      <c r="Y43" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="Z43" s="85"/>
-      <c r="AA43" s="85"/>
+      <c r="Z43" s="86"/>
+      <c r="AA43" s="86"/>
       <c r="AB43" s="21">
         <v>0.875</v>
       </c>
@@ -3371,27 +3390,27 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="20">
-        <v>44657</v>
+        <v>44661</v>
       </c>
       <c r="D44" s="12"/>
-      <c r="E44" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="85"/>
+      <c r="E44" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
       <c r="H44" s="21">
-        <v>0.375</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="I44" s="21">
-        <v>0.51527777777777783</v>
+        <v>0.78472222222222221</v>
       </c>
       <c r="J44" s="31">
         <f t="shared" si="0"/>
-        <v>0.14027777777777783</v>
+        <v>7.638888888888884E-2</v>
       </c>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
@@ -3420,11 +3439,11 @@
         <v>44666</v>
       </c>
       <c r="X44" s="12"/>
-      <c r="Y44" s="85" t="s">
+      <c r="Y44" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="Z44" s="85"/>
-      <c r="AA44" s="85"/>
+      <c r="Z44" s="86"/>
+      <c r="AA44" s="86"/>
       <c r="AB44" s="21">
         <v>0.875</v>
       </c>
@@ -3436,27 +3455,27 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="20">
-        <v>44661</v>
+        <v>44663</v>
       </c>
       <c r="D45" s="12"/>
-      <c r="E45" s="85" t="s">
-        <v>87</v>
-      </c>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
+      <c r="E45" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
       <c r="H45" s="21">
-        <v>0.70833333333333337</v>
+        <v>0.4375</v>
       </c>
       <c r="I45" s="21">
-        <v>0.78472222222222221</v>
+        <v>0.52916666666666667</v>
       </c>
       <c r="J45" s="31">
         <f t="shared" si="0"/>
-        <v>7.638888888888884E-2</v>
+        <v>9.1666666666666674E-2</v>
       </c>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
@@ -3487,11 +3506,11 @@
         <v>44667</v>
       </c>
       <c r="X45" s="12"/>
-      <c r="Y45" s="85" t="s">
+      <c r="Y45" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="85"/>
-      <c r="AA45" s="85"/>
+      <c r="Z45" s="86"/>
+      <c r="AA45" s="86"/>
       <c r="AB45" s="21">
         <v>0.875</v>
       </c>
@@ -3503,27 +3522,27 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="20">
-        <v>44663</v>
+        <v>44665</v>
       </c>
       <c r="D46" s="12"/>
-      <c r="E46" s="85" t="s">
-        <v>88</v>
-      </c>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
+      <c r="E46" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
       <c r="H46" s="21">
-        <v>0.4375</v>
+        <v>0.84166666666666667</v>
       </c>
       <c r="I46" s="21">
-        <v>0.52916666666666667</v>
+        <v>0.96875</v>
       </c>
       <c r="J46" s="31">
         <f t="shared" si="0"/>
-        <v>9.1666666666666674E-2</v>
+        <v>0.12708333333333333</v>
       </c>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
@@ -3554,11 +3573,11 @@
         <v>44668</v>
       </c>
       <c r="X46" s="12"/>
-      <c r="Y46" s="85" t="s">
+      <c r="Y46" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="Z46" s="85"/>
-      <c r="AA46" s="85"/>
+      <c r="Z46" s="86"/>
+      <c r="AA46" s="86"/>
       <c r="AB46" s="21">
         <v>0.54166666666666663</v>
       </c>
@@ -3570,27 +3589,27 @@
         <v>0.16666666666666674</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="20">
-        <v>44665</v>
-      </c>
-      <c r="D47" s="12"/>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="32">
+        <v>44667</v>
+      </c>
+      <c r="D47" s="39"/>
       <c r="E47" s="85" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F47" s="85"/>
       <c r="G47" s="85"/>
-      <c r="H47" s="21">
-        <v>0.84166666666666667</v>
-      </c>
-      <c r="I47" s="21">
-        <v>0.96875</v>
+      <c r="H47" s="29">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="I47" s="29">
+        <v>0.52777777777777779</v>
       </c>
       <c r="J47" s="31">
         <f t="shared" si="0"/>
-        <v>0.12708333333333333</v>
+        <v>0.13680555555555557</v>
       </c>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
@@ -3600,11 +3619,11 @@
       <c r="N47" s="30">
         <v>7</v>
       </c>
-      <c r="O47" s="83" t="s">
+      <c r="O47" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="P47" s="83"/>
-      <c r="Q47" s="83"/>
+      <c r="P47" s="87"/>
+      <c r="Q47" s="87"/>
       <c r="R47" s="21">
         <v>0.58333333333333337</v>
       </c>
@@ -3621,11 +3640,11 @@
         <v>44669</v>
       </c>
       <c r="X47" s="39"/>
-      <c r="Y47" s="88" t="s">
+      <c r="Y47" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="Z47" s="88"/>
-      <c r="AA47" s="88"/>
+      <c r="Z47" s="85"/>
+      <c r="AA47" s="85"/>
       <c r="AB47" s="29">
         <v>0.58333333333333337</v>
       </c>
@@ -3637,28 +3656,17 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" s="39"/>
       <c r="B48" s="39"/>
-      <c r="C48" s="32">
-        <v>44667</v>
-      </c>
+      <c r="C48" s="32"/>
       <c r="D48" s="39"/>
-      <c r="E48" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="29">
-        <v>0.39097222222222222</v>
-      </c>
-      <c r="I48" s="29">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="J48" s="31">
-        <f t="shared" si="0"/>
-        <v>0.13680555555555557</v>
-      </c>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="31"/>
       <c r="K48" s="39"/>
       <c r="L48" s="12"/>
       <c r="M48" s="20">
@@ -3667,11 +3675,11 @@
       <c r="N48" s="30">
         <v>7</v>
       </c>
-      <c r="O48" s="83" t="s">
+      <c r="O48" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="P48" s="83"/>
-      <c r="Q48" s="83"/>
+      <c r="P48" s="87"/>
+      <c r="Q48" s="87"/>
       <c r="R48" s="21">
         <v>0.70833333333333337</v>
       </c>
@@ -3693,17 +3701,17 @@
       <c r="AC48" s="29"/>
       <c r="AD48" s="31"/>
     </row>
-    <row r="49" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="31"/>
+    <row r="49" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="66"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="65"/>
       <c r="K49" s="69"/>
       <c r="L49" s="66"/>
       <c r="M49" s="67">
@@ -3712,11 +3720,11 @@
       <c r="N49" s="75">
         <v>7</v>
       </c>
-      <c r="O49" s="110" t="s">
+      <c r="O49" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="P49" s="110"/>
-      <c r="Q49" s="110"/>
+      <c r="P49" s="88"/>
+      <c r="Q49" s="88"/>
       <c r="R49" s="64">
         <v>0.9375</v>
       </c>
@@ -3738,17 +3746,30 @@
       <c r="AC49" s="64"/>
       <c r="AD49" s="65"/>
     </row>
-    <row r="50" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="66"/>
-      <c r="B50" s="66"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="66"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="65"/>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A50" s="12"/>
+      <c r="B50" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="20">
+        <v>44676</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="86"/>
+      <c r="G50" s="86"/>
+      <c r="H50" s="21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I50" s="21">
+        <v>0.40625</v>
+      </c>
+      <c r="J50" s="31">
+        <f t="shared" si="0"/>
+        <v>7.2916666666666685E-2</v>
+      </c>
       <c r="K50" s="12"/>
       <c r="L50" s="38" t="s">
         <v>10</v>
@@ -3759,11 +3780,11 @@
       <c r="N50" s="15">
         <v>42</v>
       </c>
-      <c r="O50" s="88" t="s">
+      <c r="O50" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="P50" s="88"/>
-      <c r="Q50" s="88"/>
+      <c r="P50" s="85"/>
+      <c r="Q50" s="85"/>
       <c r="R50" s="21">
         <v>0.66666666666666663</v>
       </c>
@@ -3782,11 +3803,11 @@
         <v>44676</v>
       </c>
       <c r="X50" s="39"/>
-      <c r="Y50" s="88" t="s">
+      <c r="Y50" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="Z50" s="88"/>
-      <c r="AA50" s="88"/>
+      <c r="Z50" s="85"/>
+      <c r="AA50" s="85"/>
       <c r="AB50" s="34">
         <v>0.75</v>
       </c>
@@ -3798,29 +3819,27 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" s="12"/>
-      <c r="B51" s="28" t="s">
-        <v>10</v>
-      </c>
+      <c r="B51" s="12"/>
       <c r="C51" s="20">
         <v>44676</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="85" t="s">
+      <c r="E51" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
       <c r="H51" s="21">
-        <v>0.33333333333333331</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I51" s="21">
-        <v>0.40625</v>
+        <v>0.71875</v>
       </c>
       <c r="J51" s="31">
         <f t="shared" si="0"/>
-        <v>7.2916666666666685E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
@@ -3830,11 +3849,11 @@
       <c r="N51" s="12">
         <v>42</v>
       </c>
-      <c r="O51" s="85" t="s">
+      <c r="O51" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="85"/>
+      <c r="P51" s="86"/>
+      <c r="Q51" s="86"/>
       <c r="R51" s="21">
         <v>0.75</v>
       </c>
@@ -3851,11 +3870,11 @@
         <v>44676</v>
       </c>
       <c r="X51" s="12"/>
-      <c r="Y51" s="88" t="s">
+      <c r="Y51" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="Z51" s="88"/>
-      <c r="AA51" s="88"/>
+      <c r="Z51" s="85"/>
+      <c r="AA51" s="85"/>
       <c r="AB51" s="21">
         <v>0.61111111111111105</v>
       </c>
@@ -3867,27 +3886,27 @@
         <v>9.7222222222222321E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="20">
-        <v>44676</v>
+        <v>44678</v>
       </c>
       <c r="D52" s="12"/>
-      <c r="E52" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="F52" s="85"/>
-      <c r="G52" s="85"/>
+      <c r="E52" s="86" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
       <c r="H52" s="21">
-        <v>0.64583333333333337</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="I52" s="21">
-        <v>0.71875</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="J52" s="31">
         <f t="shared" si="0"/>
-        <v>7.291666666666663E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
@@ -3897,11 +3916,11 @@
       <c r="N52" s="12">
         <v>42</v>
       </c>
-      <c r="O52" s="85" t="s">
+      <c r="O52" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="P52" s="85"/>
-      <c r="Q52" s="85"/>
+      <c r="P52" s="86"/>
+      <c r="Q52" s="86"/>
       <c r="R52" s="21">
         <v>0.875</v>
       </c>
@@ -3918,11 +3937,11 @@
         <v>44679</v>
       </c>
       <c r="X52" s="12"/>
-      <c r="Y52" s="85" t="s">
+      <c r="Y52" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="Z52" s="85"/>
-      <c r="AA52" s="85"/>
+      <c r="Z52" s="86"/>
+      <c r="AA52" s="86"/>
       <c r="AB52" s="21">
         <v>0.64583333333333337</v>
       </c>
@@ -3934,27 +3953,29 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="20">
-        <v>44678</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
+        <v>44682</v>
+      </c>
+      <c r="D53" s="12">
+        <v>42</v>
+      </c>
+      <c r="E53" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
       <c r="H53" s="21">
-        <v>0.49305555555555558</v>
+        <v>0.80763888888888891</v>
       </c>
       <c r="I53" s="21">
-        <v>0.52777777777777779</v>
+        <v>0.98958333333333337</v>
       </c>
       <c r="J53" s="31">
         <f t="shared" si="0"/>
-        <v>3.472222222222221E-2</v>
+        <v>0.18194444444444446</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
@@ -3962,11 +3983,11 @@
         <v>44683</v>
       </c>
       <c r="N53" s="15"/>
-      <c r="O53" s="85" t="s">
+      <c r="O53" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="P53" s="85"/>
-      <c r="Q53" s="85"/>
+      <c r="P53" s="86"/>
+      <c r="Q53" s="86"/>
       <c r="R53" s="21">
         <v>0.33333333333333331</v>
       </c>
@@ -3983,11 +4004,11 @@
         <v>44681</v>
       </c>
       <c r="X53" s="12"/>
-      <c r="Y53" s="85" t="s">
+      <c r="Y53" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="Z53" s="85"/>
-      <c r="AA53" s="85"/>
+      <c r="Z53" s="86"/>
+      <c r="AA53" s="86"/>
       <c r="AB53" s="21">
         <v>0.85416666666666663</v>
       </c>
@@ -3999,29 +4020,27 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="20">
-        <v>44682</v>
-      </c>
-      <c r="D54" s="12">
-        <v>42</v>
-      </c>
-      <c r="E54" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
+        <v>44683</v>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="86" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="86"/>
+      <c r="G54" s="86"/>
       <c r="H54" s="21">
-        <v>0.80763888888888891</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I54" s="21">
-        <v>0.98958333333333337</v>
+        <v>0.40625</v>
       </c>
       <c r="J54" s="31">
         <f t="shared" si="0"/>
-        <v>0.18194444444444446</v>
+        <v>7.2916666666666685E-2</v>
       </c>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
@@ -4029,11 +4048,11 @@
         <v>44685</v>
       </c>
       <c r="N54" s="15"/>
-      <c r="O54" s="85" t="s">
+      <c r="O54" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="P54" s="85"/>
-      <c r="Q54" s="85"/>
+      <c r="P54" s="86"/>
+      <c r="Q54" s="86"/>
       <c r="R54" s="21">
         <v>0.83333333333333337</v>
       </c>
@@ -4050,11 +4069,11 @@
         <v>44682</v>
       </c>
       <c r="X54" s="12"/>
-      <c r="Y54" s="85" t="s">
+      <c r="Y54" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="Z54" s="85"/>
-      <c r="AA54" s="85"/>
+      <c r="Z54" s="86"/>
+      <c r="AA54" s="86"/>
       <c r="AB54" s="21">
         <v>0.75</v>
       </c>
@@ -4066,27 +4085,27 @@
         <v>0.14583333333333337</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="20">
         <v>44683</v>
       </c>
       <c r="D55" s="12"/>
-      <c r="E55" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="F55" s="85"/>
-      <c r="G55" s="85"/>
+      <c r="E55" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" s="86"/>
+      <c r="G55" s="86"/>
       <c r="H55" s="21">
-        <v>0.33333333333333331</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I55" s="21">
-        <v>0.40625</v>
+        <v>0.71875</v>
       </c>
       <c r="J55" s="31">
         <f t="shared" si="0"/>
-        <v>7.2916666666666685E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
@@ -4094,11 +4113,11 @@
         <v>44689</v>
       </c>
       <c r="N55" s="15"/>
-      <c r="O55" s="85" t="s">
+      <c r="O55" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="P55" s="85"/>
-      <c r="Q55" s="85"/>
+      <c r="P55" s="86"/>
+      <c r="Q55" s="86"/>
       <c r="R55" s="21">
         <v>0.45833333333333331</v>
       </c>
@@ -4115,11 +4134,11 @@
         <v>44683</v>
       </c>
       <c r="X55" s="12"/>
-      <c r="Y55" s="85" t="s">
+      <c r="Y55" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="Z55" s="85"/>
-      <c r="AA55" s="85"/>
+      <c r="Z55" s="86"/>
+      <c r="AA55" s="86"/>
       <c r="AB55" s="21">
         <v>0.33333333333333331</v>
       </c>
@@ -4131,27 +4150,29 @@
         <v>7.2916666666666685E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="20">
-        <v>44683</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="85" t="s">
-        <v>48</v>
-      </c>
-      <c r="F56" s="85"/>
-      <c r="G56" s="85"/>
+        <v>44685</v>
+      </c>
+      <c r="D56" s="12">
+        <v>42</v>
+      </c>
+      <c r="E56" s="86" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="86"/>
+      <c r="G56" s="86"/>
       <c r="H56" s="21">
-        <v>0.64583333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I56" s="21">
-        <v>0.71875</v>
+        <v>0.875</v>
       </c>
       <c r="J56" s="31">
         <f t="shared" si="0"/>
-        <v>7.291666666666663E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
@@ -4159,11 +4180,11 @@
         <v>44691</v>
       </c>
       <c r="N56" s="15"/>
-      <c r="O56" s="85" t="s">
+      <c r="O56" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="P56" s="85"/>
-      <c r="Q56" s="85"/>
+      <c r="P56" s="86"/>
+      <c r="Q56" s="86"/>
       <c r="R56" s="21">
         <v>0.68402777777777779</v>
       </c>
@@ -4182,11 +4203,11 @@
       <c r="X56" s="15">
         <v>42</v>
       </c>
-      <c r="Y56" s="85" t="s">
+      <c r="Y56" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="Z56" s="85"/>
-      <c r="AA56" s="85"/>
+      <c r="Z56" s="86"/>
+      <c r="AA56" s="86"/>
       <c r="AB56" s="21">
         <v>0.66666666666666663</v>
       </c>
@@ -4198,29 +4219,29 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="20">
-        <v>44685</v>
+        <v>44688</v>
       </c>
       <c r="D57" s="12">
         <v>42</v>
       </c>
-      <c r="E57" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="F57" s="85"/>
-      <c r="G57" s="85"/>
+      <c r="E57" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="86"/>
+      <c r="G57" s="86"/>
       <c r="H57" s="21">
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="I57" s="21">
-        <v>0.875</v>
+        <v>0.68611111111111101</v>
       </c>
       <c r="J57" s="31">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>6.1111111111111005E-2</v>
       </c>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
@@ -4228,11 +4249,11 @@
         <v>44692</v>
       </c>
       <c r="N57" s="15"/>
-      <c r="O57" s="85" t="s">
+      <c r="O57" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="P57" s="85"/>
-      <c r="Q57" s="85"/>
+      <c r="P57" s="86"/>
+      <c r="Q57" s="86"/>
       <c r="R57" s="21">
         <v>0.49305555555555558</v>
       </c>
@@ -4249,11 +4270,11 @@
         <v>44689</v>
       </c>
       <c r="X57" s="15"/>
-      <c r="Y57" s="85" t="s">
+      <c r="Y57" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="Z57" s="85"/>
-      <c r="AA57" s="85"/>
+      <c r="Z57" s="86"/>
+      <c r="AA57" s="86"/>
       <c r="AB57" s="21">
         <v>0.45833333333333331</v>
       </c>
@@ -4265,29 +4286,27 @@
         <v>7.2916666666666685E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="12"/>
       <c r="B58" s="12"/>
       <c r="C58" s="20">
-        <v>44688</v>
-      </c>
-      <c r="D58" s="12">
-        <v>42</v>
-      </c>
-      <c r="E58" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="85"/>
-      <c r="G58" s="85"/>
+        <v>44689</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" s="86"/>
+      <c r="G58" s="86"/>
       <c r="H58" s="21">
-        <v>0.625</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="I58" s="21">
-        <v>0.68611111111111101</v>
+        <v>0.53125</v>
       </c>
       <c r="J58" s="31">
         <f t="shared" si="0"/>
-        <v>6.1111111111111005E-2</v>
+        <v>7.2916666666666685E-2</v>
       </c>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
@@ -4295,11 +4314,11 @@
         <v>44695</v>
       </c>
       <c r="N58" s="12"/>
-      <c r="O58" s="85" t="s">
+      <c r="O58" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="P58" s="85"/>
-      <c r="Q58" s="85"/>
+      <c r="P58" s="86"/>
+      <c r="Q58" s="86"/>
       <c r="R58" s="21">
         <v>0.54166666666666663</v>
       </c>
@@ -4316,11 +4335,11 @@
         <v>44691</v>
       </c>
       <c r="X58" s="12"/>
-      <c r="Y58" s="85" t="s">
+      <c r="Y58" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="Z58" s="85"/>
-      <c r="AA58" s="85"/>
+      <c r="Z58" s="86"/>
+      <c r="AA58" s="86"/>
       <c r="AB58" s="21">
         <v>0.875</v>
       </c>
@@ -4332,27 +4351,27 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" s="12"/>
       <c r="B59" s="12"/>
       <c r="C59" s="20">
-        <v>44689</v>
+        <v>44691</v>
       </c>
       <c r="D59" s="12"/>
-      <c r="E59" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
+      <c r="E59" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="86"/>
+      <c r="G59" s="86"/>
       <c r="H59" s="21">
-        <v>0.45833333333333331</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="I59" s="21">
-        <v>0.53125</v>
+        <v>0.71875</v>
       </c>
       <c r="J59" s="31">
         <f t="shared" si="0"/>
-        <v>7.2916666666666685E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
@@ -4360,11 +4379,11 @@
         <v>44695</v>
       </c>
       <c r="N59" s="12"/>
-      <c r="O59" s="85" t="s">
+      <c r="O59" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="P59" s="85"/>
-      <c r="Q59" s="85"/>
+      <c r="P59" s="86"/>
+      <c r="Q59" s="86"/>
       <c r="R59" s="21">
         <v>0.75</v>
       </c>
@@ -4381,11 +4400,11 @@
         <v>44696</v>
       </c>
       <c r="X59" s="12"/>
-      <c r="Y59" s="85" t="s">
+      <c r="Y59" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="Z59" s="85"/>
-      <c r="AA59" s="85"/>
+      <c r="Z59" s="86"/>
+      <c r="AA59" s="86"/>
       <c r="AB59" s="21">
         <v>0.625</v>
       </c>
@@ -4397,23 +4416,25 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" s="12"/>
       <c r="B60" s="12"/>
       <c r="C60" s="20">
-        <v>44691</v>
-      </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="85" t="s">
+        <v>44692</v>
+      </c>
+      <c r="D60" s="12">
+        <v>42</v>
+      </c>
+      <c r="E60" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="F60" s="85"/>
-      <c r="G60" s="85"/>
+      <c r="F60" s="86"/>
+      <c r="G60" s="86"/>
       <c r="H60" s="21">
-        <v>0.68402777777777779</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="I60" s="21">
-        <v>0.71875</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="J60" s="31">
         <f t="shared" si="0"/>
@@ -4425,11 +4446,11 @@
         <v>44696</v>
       </c>
       <c r="N60" s="12"/>
-      <c r="O60" s="85" t="s">
+      <c r="O60" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="P60" s="85"/>
-      <c r="Q60" s="85"/>
+      <c r="P60" s="86"/>
+      <c r="Q60" s="86"/>
       <c r="R60" s="21">
         <v>0.625</v>
       </c>
@@ -4444,36 +4465,34 @@
       <c r="V60" s="12"/>
       <c r="W60" s="20"/>
       <c r="X60" s="12"/>
-      <c r="Y60" s="85"/>
-      <c r="Z60" s="85"/>
-      <c r="AA60" s="85"/>
+      <c r="Y60" s="86"/>
+      <c r="Z60" s="86"/>
+      <c r="AA60" s="86"/>
       <c r="AB60" s="21"/>
       <c r="AC60" s="21"/>
       <c r="AD60" s="31"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="12"/>
       <c r="B61" s="12"/>
       <c r="C61" s="20">
-        <v>44692</v>
-      </c>
-      <c r="D61" s="12">
-        <v>42</v>
-      </c>
-      <c r="E61" s="85" t="s">
-        <v>98</v>
-      </c>
-      <c r="F61" s="85"/>
-      <c r="G61" s="85"/>
+        <v>44695</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="86"/>
+      <c r="G61" s="86"/>
       <c r="H61" s="21">
-        <v>0.49305555555555558</v>
+        <v>0.77222222222222225</v>
       </c>
       <c r="I61" s="21">
-        <v>0.52777777777777779</v>
+        <v>0.8652777777777777</v>
       </c>
       <c r="J61" s="31">
         <f t="shared" si="0"/>
-        <v>3.472222222222221E-2</v>
+        <v>9.3055555555555447E-2</v>
       </c>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
@@ -4481,11 +4500,11 @@
         <v>44696</v>
       </c>
       <c r="N61" s="12"/>
-      <c r="O61" s="85" t="s">
+      <c r="O61" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="P61" s="85"/>
-      <c r="Q61" s="85"/>
+      <c r="P61" s="86"/>
+      <c r="Q61" s="86"/>
       <c r="R61" s="21">
         <v>0.9375</v>
       </c>
@@ -4499,34 +4518,34 @@
       <c r="V61" s="12"/>
       <c r="W61" s="12"/>
       <c r="X61" s="12"/>
-      <c r="Y61" s="85"/>
-      <c r="Z61" s="85"/>
-      <c r="AA61" s="85"/>
+      <c r="Y61" s="86"/>
+      <c r="Z61" s="86"/>
+      <c r="AA61" s="86"/>
       <c r="AB61" s="12"/>
       <c r="AC61" s="12"/>
       <c r="AD61" s="31"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="20">
-        <v>44695</v>
-      </c>
-      <c r="D62" s="12"/>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A62" s="81"/>
+      <c r="B62" s="81"/>
+      <c r="C62" s="32">
+        <v>44696</v>
+      </c>
+      <c r="D62" s="83"/>
       <c r="E62" s="85" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F62" s="85"/>
       <c r="G62" s="85"/>
-      <c r="H62" s="21">
-        <v>0.77222222222222225</v>
-      </c>
-      <c r="I62" s="21">
-        <v>0.8652777777777777</v>
+      <c r="H62" s="29">
+        <v>0.7909722222222223</v>
+      </c>
+      <c r="I62" s="29">
+        <v>0.90555555555555556</v>
       </c>
       <c r="J62" s="31">
-        <f t="shared" si="0"/>
-        <v>9.3055555555555447E-2</v>
+        <f t="shared" ref="J62" si="9">I62-H62</f>
+        <v>0.11458333333333326</v>
       </c>
       <c r="K62" s="40"/>
       <c r="L62" s="40"/>
@@ -4549,35 +4568,24 @@
       <c r="AC62" s="40"/>
       <c r="AD62" s="31"/>
     </row>
-    <row r="63" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="66"/>
       <c r="B63" s="66"/>
-      <c r="C63" s="67">
-        <v>44696</v>
-      </c>
+      <c r="C63" s="67"/>
       <c r="D63" s="66"/>
-      <c r="E63" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="F63" s="87"/>
-      <c r="G63" s="87"/>
-      <c r="H63" s="64">
-        <v>0.7909722222222223</v>
-      </c>
-      <c r="I63" s="64">
-        <v>0.90555555555555556</v>
-      </c>
-      <c r="J63" s="65">
-        <f t="shared" si="0"/>
-        <v>0.11458333333333326</v>
-      </c>
+      <c r="E63" s="93"/>
+      <c r="F63" s="93"/>
+      <c r="G63" s="93"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="64"/>
+      <c r="J63" s="65"/>
       <c r="K63" s="49"/>
       <c r="L63" s="49"/>
       <c r="M63" s="49"/>
       <c r="N63" s="49"/>
-      <c r="O63" s="86"/>
-      <c r="P63" s="86"/>
-      <c r="Q63" s="86"/>
+      <c r="O63" s="112"/>
+      <c r="P63" s="112"/>
+      <c r="Q63" s="112"/>
       <c r="R63" s="49"/>
       <c r="S63" s="49"/>
       <c r="T63" s="51"/>
@@ -4592,18 +4600,18 @@
       <c r="AC63" s="66"/>
       <c r="AD63" s="74"/>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C64" s="35">
         <v>44704</v>
       </c>
-      <c r="E64" s="84" t="s">
+      <c r="E64" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="F64" s="84"/>
-      <c r="G64" s="84"/>
+      <c r="F64" s="111"/>
+      <c r="G64" s="111"/>
       <c r="H64" s="36">
         <v>0.33333333333333331</v>
       </c>
@@ -4623,18 +4631,18 @@
       <c r="N64">
         <v>49.51</v>
       </c>
-      <c r="O64" s="83" t="s">
+      <c r="O64" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="P64" s="83"/>
-      <c r="Q64" s="83"/>
+      <c r="P64" s="87"/>
+      <c r="Q64" s="87"/>
       <c r="R64" s="36">
         <v>0.70833333333333337</v>
       </c>
       <c r="S64" s="36">
         <v>0.77361111111111114</v>
       </c>
-      <c r="T64" s="80">
+      <c r="T64" s="113">
         <f>S64-R64</f>
         <v>6.5277777777777768E-2</v>
       </c>
@@ -4645,11 +4653,11 @@
       <c r="W64" s="35">
         <v>44701</v>
       </c>
-      <c r="Y64" s="84" t="s">
+      <c r="Y64" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="Z64" s="84"/>
-      <c r="AA64" s="84"/>
+      <c r="Z64" s="111"/>
+      <c r="AA64" s="111"/>
       <c r="AB64" s="36">
         <v>0.75</v>
       </c>
@@ -4661,16 +4669,16 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="65" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C65" s="35">
         <v>44704</v>
       </c>
       <c r="D65" s="37"/>
-      <c r="E65" s="83" t="s">
+      <c r="E65" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="F65" s="83"/>
-      <c r="G65" s="83"/>
+      <c r="F65" s="87"/>
+      <c r="G65" s="87"/>
       <c r="H65" s="36">
         <v>0.64583333333333337</v>
       </c>
@@ -4687,18 +4695,18 @@
       <c r="N65">
         <v>49.51</v>
       </c>
-      <c r="O65" s="83" t="s">
+      <c r="O65" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="P65" s="83"/>
-      <c r="Q65" s="83"/>
+      <c r="P65" s="87"/>
+      <c r="Q65" s="87"/>
       <c r="R65" s="36">
         <v>0.48958333333333331</v>
       </c>
       <c r="S65" s="36">
         <v>0.53125</v>
       </c>
-      <c r="T65" s="81">
+      <c r="T65" s="48">
         <f>SUM(S65-R65)</f>
         <v>4.1666666666666685E-2</v>
       </c>
@@ -4708,11 +4716,11 @@
         <v>44704</v>
       </c>
       <c r="X65" s="37"/>
-      <c r="Y65" s="83" t="s">
+      <c r="Y65" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="Z65" s="83"/>
-      <c r="AA65" s="83"/>
+      <c r="Z65" s="87"/>
+      <c r="AA65" s="87"/>
       <c r="AB65" s="36">
         <v>0.64583333333333337</v>
       </c>
@@ -4724,16 +4732,16 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="66" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C66" s="35">
         <v>44706</v>
       </c>
       <c r="D66" s="37"/>
-      <c r="E66" s="83" t="s">
+      <c r="E66" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="F66" s="83"/>
-      <c r="G66" s="83"/>
+      <c r="F66" s="87"/>
+      <c r="G66" s="87"/>
       <c r="H66" s="36">
         <v>0.48958333333333331</v>
       </c>
@@ -4750,18 +4758,18 @@
       <c r="N66">
         <v>49.51</v>
       </c>
-      <c r="O66" s="83" t="s">
+      <c r="O66" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="P66" s="83"/>
-      <c r="Q66" s="83"/>
+      <c r="P66" s="87"/>
+      <c r="Q66" s="87"/>
       <c r="R66" s="36">
         <v>0.64583333333333337</v>
       </c>
       <c r="S66" s="36">
         <v>0.83124999999999993</v>
       </c>
-      <c r="T66" s="81">
+      <c r="T66" s="48">
         <f>SUM(S66-R66)</f>
         <v>0.18541666666666656</v>
       </c>
@@ -4772,10 +4780,10 @@
       </c>
       <c r="X66" s="37"/>
       <c r="Y66" s="37"/>
-      <c r="Z66" s="82" t="s">
+      <c r="Z66" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="AA66" s="82"/>
+      <c r="AA66" s="80"/>
       <c r="AB66" s="36">
         <v>0.7090277777777777</v>
       </c>
@@ -4787,7 +4795,7 @@
         <v>0.13125000000000009</v>
       </c>
     </row>
-    <row r="67" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C67" s="35">
         <v>44709</v>
       </c>
@@ -4813,18 +4821,18 @@
       <c r="N67">
         <v>49.51</v>
       </c>
-      <c r="O67" s="83" t="s">
+      <c r="O67" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="P67" s="83"/>
-      <c r="Q67" s="83"/>
+      <c r="P67" s="87"/>
+      <c r="Q67" s="87"/>
       <c r="R67" s="36">
         <v>0.70833333333333337</v>
       </c>
       <c r="S67" s="36">
         <v>0.8125</v>
       </c>
-      <c r="T67" s="81">
+      <c r="T67" s="48">
         <f>SUM(S67-R67)</f>
         <v>0.10416666666666663</v>
       </c>
@@ -4835,10 +4843,10 @@
       </c>
       <c r="X67" s="37"/>
       <c r="Y67" s="37"/>
-      <c r="Z67" s="82" t="s">
+      <c r="Z67" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="AA67" s="82"/>
+      <c r="AA67" s="80"/>
       <c r="AB67" s="36">
         <v>0.66666666666666663</v>
       </c>
@@ -4850,7 +4858,7 @@
         <v>0.22916666666666674</v>
       </c>
     </row>
-    <row r="68" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C68" s="35">
         <v>44710</v>
       </c>
@@ -4876,18 +4884,18 @@
       <c r="N68">
         <v>49.51</v>
       </c>
-      <c r="O68" s="83" t="s">
+      <c r="O68" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="P68" s="83"/>
-      <c r="Q68" s="83"/>
+      <c r="P68" s="87"/>
+      <c r="Q68" s="87"/>
       <c r="R68" s="36">
         <v>0.65277777777777779</v>
       </c>
       <c r="S68" s="36">
         <v>0.80208333333333337</v>
       </c>
-      <c r="T68" s="81">
+      <c r="T68" s="48">
         <f>SUM(S68-R68)</f>
         <v>0.14930555555555558</v>
       </c>
@@ -4895,11 +4903,11 @@
         <v>44712</v>
       </c>
       <c r="X68" s="39"/>
-      <c r="Y68" s="88" t="s">
+      <c r="Y68" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="Z68" s="88"/>
-      <c r="AA68" s="88"/>
+      <c r="Z68" s="85"/>
+      <c r="AA68" s="85"/>
       <c r="AB68" s="29">
         <v>0.79166666666666663</v>
       </c>
@@ -4911,15 +4919,15 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="69" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C69" s="35">
         <v>44710</v>
       </c>
-      <c r="E69" s="85" t="s">
+      <c r="E69" s="86" t="s">
         <v>125</v>
       </c>
-      <c r="F69" s="85"/>
-      <c r="G69" s="85"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
       <c r="H69" s="36">
         <v>0.89583333333333337</v>
       </c>
@@ -4936,52 +4944,199 @@
       <c r="N69">
         <v>49.51</v>
       </c>
-      <c r="O69" s="83" t="s">
+      <c r="O69" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="P69" s="83"/>
-      <c r="Q69" s="83"/>
+      <c r="P69" s="87"/>
+      <c r="Q69" s="87"/>
       <c r="R69" s="36">
         <v>0.82638888888888884</v>
       </c>
       <c r="S69" s="36">
         <v>0.94444444444444453</v>
       </c>
-      <c r="T69" s="81">
+      <c r="T69" s="48">
         <f>SUM(S69-R69)</f>
         <v>0.11805555555555569</v>
       </c>
       <c r="AD69" s="53"/>
     </row>
-    <row r="70" spans="3:30" x14ac:dyDescent="0.2">
-      <c r="J70" s="53"/>
-      <c r="L70" s="1" t="s">
+    <row r="70" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="82"/>
+      <c r="B70" s="82"/>
+      <c r="C70" s="82"/>
+      <c r="D70" s="82"/>
+      <c r="E70" s="82"/>
+      <c r="F70" s="82"/>
+      <c r="G70" s="82"/>
+      <c r="H70" s="82"/>
+      <c r="I70" s="82"/>
+      <c r="J70" s="51"/>
+      <c r="K70" s="82"/>
+      <c r="L70" s="82"/>
+      <c r="M70" s="115"/>
+      <c r="N70" s="82"/>
+      <c r="O70" s="84"/>
+      <c r="P70" s="84"/>
+      <c r="Q70" s="84"/>
+      <c r="R70" s="116"/>
+      <c r="S70" s="116"/>
+      <c r="T70" s="117"/>
+      <c r="U70" s="114"/>
+      <c r="V70" s="82"/>
+      <c r="W70" s="82"/>
+      <c r="X70" s="82"/>
+      <c r="Y70" s="82"/>
+      <c r="Z70" s="82"/>
+      <c r="AA70" s="82"/>
+      <c r="AB70" s="82"/>
+      <c r="AC70" s="82"/>
+      <c r="AD70" s="51"/>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J71" s="53"/>
+      <c r="L71" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M70" s="35">
+      <c r="M71" s="35">
         <v>44711</v>
       </c>
-      <c r="O70" s="83" t="s">
+      <c r="O71" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="P70" s="83"/>
-      <c r="Q70" s="83"/>
-      <c r="R70" s="36">
+      <c r="P71" s="87"/>
+      <c r="Q71" s="87"/>
+      <c r="R71" s="36">
         <v>0.5</v>
       </c>
-      <c r="S70" s="36">
+      <c r="S71" s="36">
         <v>0.60416666666666663</v>
       </c>
-      <c r="T70" s="81">
+      <c r="T71" s="113">
         <v>0.10416666666666667</v>
       </c>
-      <c r="AD70" s="53"/>
-    </row>
-    <row r="71" spans="3:30" x14ac:dyDescent="0.2">
       <c r="AA71" s="5"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J72" s="53"/>
+      <c r="T72" s="53"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J73" s="53"/>
+      <c r="T73" s="53"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J74" s="53"/>
+      <c r="T74" s="53"/>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J75" s="53"/>
+      <c r="T75" s="53"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J76" s="53"/>
+      <c r="T76" s="53"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="T77" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="119">
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="O68:Q68"/>
+    <mergeCell ref="O69:Q69"/>
+    <mergeCell ref="O71:Q71"/>
+    <mergeCell ref="Y57:AA57"/>
+    <mergeCell ref="O61:Q61"/>
+    <mergeCell ref="O63:Q63"/>
+    <mergeCell ref="O64:Q64"/>
+    <mergeCell ref="O65:Q65"/>
+    <mergeCell ref="O66:Q66"/>
+    <mergeCell ref="Y65:AA65"/>
+    <mergeCell ref="Y68:AA68"/>
+    <mergeCell ref="Y64:AA64"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="O57:Q57"/>
+    <mergeCell ref="O58:Q58"/>
+    <mergeCell ref="O59:Q59"/>
+    <mergeCell ref="O60:Q60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="Y46:AA46"/>
+    <mergeCell ref="Y32:AA32"/>
+    <mergeCell ref="Y34:AA34"/>
+    <mergeCell ref="Y43:AA43"/>
+    <mergeCell ref="Y33:AA33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="Y36:AA36"/>
+    <mergeCell ref="Y37:AA37"/>
+    <mergeCell ref="Y38:AA38"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="Y42:AA42"/>
+    <mergeCell ref="Y40:AA40"/>
+    <mergeCell ref="Y41:AA41"/>
     <mergeCell ref="Y50:AA50"/>
     <mergeCell ref="Y51:AA51"/>
     <mergeCell ref="Y52:AA52"/>
@@ -5006,101 +5161,6 @@
     <mergeCell ref="O55:Q55"/>
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="Y45:AA45"/>
-    <mergeCell ref="Y46:AA46"/>
-    <mergeCell ref="Y32:AA32"/>
-    <mergeCell ref="Y34:AA34"/>
-    <mergeCell ref="Y43:AA43"/>
-    <mergeCell ref="Y33:AA33"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="Y36:AA36"/>
-    <mergeCell ref="Y37:AA37"/>
-    <mergeCell ref="Y38:AA38"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="Y42:AA42"/>
-    <mergeCell ref="Y40:AA40"/>
-    <mergeCell ref="Y41:AA41"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="O56:Q56"/>
-    <mergeCell ref="O57:Q57"/>
-    <mergeCell ref="O58:Q58"/>
-    <mergeCell ref="O59:Q59"/>
-    <mergeCell ref="O60:Q60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="O67:Q67"/>
-    <mergeCell ref="O68:Q68"/>
-    <mergeCell ref="O69:Q69"/>
-    <mergeCell ref="O70:Q70"/>
-    <mergeCell ref="Y57:AA57"/>
-    <mergeCell ref="O61:Q61"/>
-    <mergeCell ref="O63:Q63"/>
-    <mergeCell ref="O64:Q64"/>
-    <mergeCell ref="O65:Q65"/>
-    <mergeCell ref="O66:Q66"/>
-    <mergeCell ref="Y65:AA65"/>
-    <mergeCell ref="Y68:AA68"/>
-    <mergeCell ref="Y64:AA64"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>